<commit_message>
Cambio en la respuesta delete para traerlo desde la data de excel
</commit_message>
<xml_diff>
--- a/build/resources/main/Data/DataUser.xlsx
+++ b/build/resources/main/Data/DataUser.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">FIRSTNAME</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">CODE</t>
   </si>
   <si>
+    <t xml:space="preserve">RESPONSE_PHONE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Esteban</t>
   </si>
   <si>
@@ -62,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">/users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-570-236-7033</t>
   </si>
 </sst>
 </file>
@@ -151,7 +157,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,16 +178,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -206,34 +213,40 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>3102809872</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="n">
         <v>200</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>